<commit_message>
readey to change file_reader it's a backup
</commit_message>
<xml_diff>
--- a/classes.xlsx
+++ b/classes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\python\graduation_design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2C9781-D7B7-4F94-9791-665AE3C145D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF1A6EE-FB59-4562-9AA8-FAAF98F7D9C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15690" xr2:uid="{BE775438-F8B0-4D04-953A-221A3496657E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15930" xr2:uid="{BE775438-F8B0-4D04-953A-221A3496657E}"/>
   </bookViews>
   <sheets>
     <sheet name="类设计图" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="121">
   <si>
     <t>属性</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -54,10 +54,6 @@
   </si>
   <si>
     <t xml:space="preserve">open_file_btn_clicked </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&gt;处理display_file_name_label</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -317,10 +313,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>icon_btn_double_clicked_handler</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>&gt;File_Reader_Dialog</t>
   </si>
   <si>
@@ -328,10 +320,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>start</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Light_Label(QLabel)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -352,14 +340,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>新建信号_double_clicked</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MainWindow</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>qt_scrollarea_viewport</t>
   </si>
   <si>
@@ -375,6 +355,157 @@
   </si>
   <si>
     <t>Function_widget</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Draw_Scroll_Area_Content</t>
+  </si>
+  <si>
+    <t>get_function_widget()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>function_widget_set</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt; 画布上的所有function widget</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Curve</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>function_widget</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt; curve依附的function widget</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>start_point</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>end_point</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>start_label</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>end_label</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>end_label_moved_handler(x, y)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>paintEvent()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mousePressEvent()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>resizeEvent()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>moveEvent()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>End_Label</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt; end_label拖动的时候发射</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mouseMoveEvent(）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>moved_signal(int, int)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;将鼠标相对于屏幕原点的坐标，发送给end_label_moved_handler(x, y)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mouseReleaseEvent()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt; 判断当前end_label鼠标放下的时候，是否处于某个function widget里面，然后关联不同的function widget</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>class_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>next_widget</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>previous_widget</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>state_changed_handler("state")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;当控件移动的时候，判断有没有关联的控件，然后调整curve的位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get_left_sucket()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;获取控件左边按钮的位置作为curve的end_point</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;改变light_label的颜色</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>icon_btn_double_clicked_handler()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>self.dataFrame</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;储存dialog里面的数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>display_table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;这个函数里面读取数据，并保存在File_Reader_Dilog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;处理open_file_btn真正选中一个文件之后的文件路径</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新建信号 double_clicked</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -527,26 +658,8 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -558,14 +671,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -881,263 +1018,435 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13571FCC-B3EF-4161-ABD1-4E93E3CEDD5C}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.75" customWidth="1"/>
+    <col min="1" max="1" width="25.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="3"/>
+    <col min="4" max="4" width="18.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9" style="3"/>
+    <col min="8" max="8" width="37.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.75" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="D1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="14"/>
+      <c r="H1" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="14"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H8" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="I8" s="14"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="D1" s="10" t="s">
+      <c r="B9" s="14"/>
+      <c r="D9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="H9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="H1" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="I1" s="11"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="B11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H11" s="8"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="6"/>
+      <c r="B14" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="I14" s="12"/>
+    </row>
+    <row r="15" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="6"/>
+      <c r="B15" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="I15" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+    </row>
+    <row r="16" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D17" s="6"/>
+      <c r="E17" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D18" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D19" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="7"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D20" s="6"/>
+      <c r="E20" s="7"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D21" s="8"/>
+      <c r="E21" s="9"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D25" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="14"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D26" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E26" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H26" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="I26" s="14"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D27" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="H27" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I27" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="2" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D28" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" s="7"/>
+      <c r="H28" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D29" s="8"/>
+      <c r="E29" s="9"/>
+      <c r="H29" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H30" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H32" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H8" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="I8" s="11"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="11"/>
-      <c r="D9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="11"/>
-      <c r="H9" s="5" t="s">
+      <c r="B33" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="I33" s="9"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="I37" s="14"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H38" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I38" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D15" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H17" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="I17" s="12"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D19" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="11"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D20" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D22" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D23" s="2"/>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>83</v>
-      </c>
-      <c r="B31" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>86</v>
-      </c>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H39" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="H40" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H41" s="6"/>
+      <c r="I41" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="57" x14ac:dyDescent="0.2">
+      <c r="H42" s="6"/>
+      <c r="I42" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H43" s="8"/>
+      <c r="I43" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H17:I17"/>
+  <mergeCells count="9">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="D9:E9"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H8:I8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1163,203 +1472,203 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="8">
+        <v>35</v>
+      </c>
+      <c r="F2" s="2">
         <v>8.9109999999999996</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="8" t="s">
         <v>55</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="8">
+        <v>22</v>
+      </c>
+      <c r="F4" s="2">
         <v>11.048</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
-        <v>50</v>
+      <c r="A5" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="8">
+        <v>22</v>
+      </c>
+      <c r="F5" s="2">
         <v>35.386000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="8">
+        <v>22</v>
+      </c>
+      <c r="F6" s="2">
         <v>23.239000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="9" t="s">
         <v>42</v>
       </c>
+      <c r="B7" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="8">
+        <v>35</v>
+      </c>
+      <c r="F8" s="2">
         <v>7.3540000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="8" t="s">
         <v>30</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="8">
+        <v>22</v>
+      </c>
+      <c r="F10" s="2">
         <v>11.878</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="7">
+        <v>22</v>
+      </c>
+      <c r="F11" s="1">
         <v>11.878</v>
       </c>
     </row>

</xml_diff>